<commit_message>
fix everything is working correct
</commit_message>
<xml_diff>
--- a/src/data/BuscarProductoData.xlsx
+++ b/src/data/BuscarProductoData.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/veliz/Development/workspace-vscode-macbookpro/workspace-201901/workspace-isw/bodeguita/bodeguita-test/src/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02BA6644-24A9-6C4E-8654-D67246E69E0F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="10410"/>
+    <workbookView xWindow="9920" yWindow="9780" windowWidth="20740" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -14,11 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -56,16 +57,16 @@
     <t>Buscar Categoría - Criterio Aceptación 01</t>
   </si>
   <si>
-    <t>http://localhost:8080/BodeWeb</t>
-  </si>
-  <si>
     <t>Galleta Casino Clásica</t>
+  </si>
+  <si>
+    <t>http://localhost:3000/auth</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -124,12 +125,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,34 +436,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection sqref="A1:F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="49.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="49.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -483,12 +483,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>10</v>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>1</v>
@@ -497,18 +497,18 @@
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="3">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>10</v>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
@@ -525,8 +525,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="http://localhost:8080/VisorWeb"/>
-    <hyperlink ref="B3" r:id="rId2" display="http://localhost:8080/VisorWeb"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{A5271966-B6BF-9642-8BFF-AAAA25AC6602}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{17C2C124-1271-C445-BCD5-565D3EDD565C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>